<commit_message>
Modified get_twitter_info function. It is using twitter website instead of Socialblade. Updated the multithread funstions and improved execution time
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="660">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1132" uniqueCount="719">
   <si>
     <t>Contact Name</t>
   </si>
@@ -1802,25 +1802,55 @@
     <t>https://www.youtube.com/channel/Japan</t>
   </si>
   <si>
-    <t>2238</t>
-  </si>
-  <si>
-    <t>2028</t>
+    <t>2239</t>
+  </si>
+  <si>
+    <t>2031</t>
   </si>
   <si>
     <t>1844</t>
   </si>
   <si>
-    <t>3866</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>5.61M</t>
-  </si>
-  <si>
-    <t>2.44M</t>
+    <t>3869</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>1623</t>
+  </si>
+  <si>
+    <t>1123</t>
+  </si>
+  <si>
+    <t>1228</t>
+  </si>
+  <si>
+    <t>217</t>
+  </si>
+  <si>
+    <t>335</t>
+  </si>
+  <si>
+    <t>537</t>
+  </si>
+  <si>
+    <t>166</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>3958</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>5.62M</t>
+  </si>
+  <si>
+    <t>2.46M</t>
   </si>
   <si>
     <t>1.78M</t>
@@ -1829,43 +1859,82 @@
     <t>1.46M</t>
   </si>
   <si>
-    <t>251K</t>
-  </si>
-  <si>
-    <t>3899243060</t>
-  </si>
-  <si>
-    <t>2548759255</t>
-  </si>
-  <si>
-    <t>1358716007</t>
-  </si>
-  <si>
-    <t>858396934</t>
-  </si>
-  <si>
-    <t>46085617</t>
-  </si>
-  <si>
-    <t>72,548,736</t>
-  </si>
-  <si>
-    <t>101,143,195</t>
-  </si>
-  <si>
-    <t>59,523,888</t>
-  </si>
-  <si>
-    <t>24,319,728</t>
-  </si>
-  <si>
-    <t>19,751,889</t>
-  </si>
-  <si>
-    <t>33,831,183</t>
-  </si>
-  <si>
-    <t>9,595,182</t>
+    <t>253K</t>
+  </si>
+  <si>
+    <t>143K</t>
+  </si>
+  <si>
+    <t>96.9K</t>
+  </si>
+  <si>
+    <t>53.9K</t>
+  </si>
+  <si>
+    <t>93K</t>
+  </si>
+  <si>
+    <t>55K</t>
+  </si>
+  <si>
+    <t>42.2K</t>
+  </si>
+  <si>
+    <t>50.8K</t>
+  </si>
+  <si>
+    <t>32.9K</t>
+  </si>
+  <si>
+    <t>101M</t>
+  </si>
+  <si>
+    <t>1.15K</t>
+  </si>
+  <si>
+    <t>3903113533</t>
+  </si>
+  <si>
+    <t>2552677239</t>
+  </si>
+  <si>
+    <t>1359421232</t>
+  </si>
+  <si>
+    <t>859283273</t>
+  </si>
+  <si>
+    <t>46542627</t>
+  </si>
+  <si>
+    <t>72626322</t>
+  </si>
+  <si>
+    <t>101237916</t>
+  </si>
+  <si>
+    <t>59753446</t>
+  </si>
+  <si>
+    <t>25555069</t>
+  </si>
+  <si>
+    <t>19657263</t>
+  </si>
+  <si>
+    <t>33873652</t>
+  </si>
+  <si>
+    <t>10271855</t>
+  </si>
+  <si>
+    <t>8866893</t>
+  </si>
+  <si>
+    <t>23474006016</t>
+  </si>
+  <si>
+    <t>330218</t>
   </si>
   <si>
     <t>https://www.instagram.com/teamawesmr/</t>
@@ -1898,7 +1967,7 @@
     <t>https://www.instagram.com/hazarblablabla/</t>
   </si>
   <si>
-    <t>111</t>
+    <t>114</t>
   </si>
   <si>
     <t>289</t>
@@ -1907,13 +1976,55 @@
     <t>85</t>
   </si>
   <si>
-    <t>42.2k</t>
+    <t>1,018</t>
+  </si>
+  <si>
+    <t>1,278</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>275</t>
+  </si>
+  <si>
+    <t>1,153</t>
+  </si>
+  <si>
+    <t>265</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>42.6k</t>
   </si>
   <si>
     <t>27.2k</t>
   </si>
   <si>
-    <t>1,246</t>
+    <t>1,249</t>
+  </si>
+  <si>
+    <t>1,066</t>
+  </si>
+  <si>
+    <t>2,332</t>
+  </si>
+  <si>
+    <t>134</t>
+  </si>
+  <si>
+    <t>1,323</t>
+  </si>
+  <si>
+    <t>1,114</t>
+  </si>
+  <si>
+    <t>762</t>
+  </si>
+  <si>
+    <t>154</t>
   </si>
   <si>
     <t>0</t>
@@ -1922,7 +2033,28 @@
     <t>38</t>
   </si>
   <si>
-    <t>2,324</t>
+    <t>2,325</t>
+  </si>
+  <si>
+    <t>69</t>
+  </si>
+  <si>
+    <t>5,780</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>485</t>
+  </si>
+  <si>
+    <t>391</t>
+  </si>
+  <si>
+    <t>333</t>
+  </si>
+  <si>
+    <t>200</t>
   </si>
   <si>
     <t>https://twitter.com/teamAWESMR</t>
@@ -1949,22 +2081,43 @@
     <t>https://twitter.com/PlanettSerenity</t>
   </si>
   <si>
-    <t>1,058</t>
-  </si>
-  <si>
-    <t>1,966</t>
-  </si>
-  <si>
-    <t>962</t>
+    <t>1058</t>
+  </si>
+  <si>
+    <t>1963</t>
+  </si>
+  <si>
+    <t>960</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>658</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>796</t>
+  </si>
+  <si>
+    <t>706</t>
   </si>
   <si>
     <t>57</t>
   </si>
   <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>725</t>
+    <t>727</t>
+  </si>
+  <si>
+    <t>1403</t>
+  </si>
+  <si>
+    <t>259</t>
+  </si>
+  <si>
+    <t>141</t>
   </si>
   <si>
     <t>10</t>
@@ -1973,16 +2126,40 @@
     <t>12</t>
   </si>
   <si>
-    <t>1,527</t>
-  </si>
-  <si>
-    <t>2,049</t>
-  </si>
-  <si>
-    <t>4,136</t>
-  </si>
-  <si>
-    <t>1,129</t>
+    <t>1530</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>137</t>
+  </si>
+  <si>
+    <t>467</t>
+  </si>
+  <si>
+    <t>548</t>
+  </si>
+  <si>
+    <t>2049</t>
+  </si>
+  <si>
+    <t>4136</t>
+  </si>
+  <si>
+    <t>1130</t>
+  </si>
+  <si>
+    <t>8328</t>
+  </si>
+  <si>
+    <t>775</t>
+  </si>
+  <si>
+    <t>282</t>
+  </si>
+  <si>
+    <t>1006</t>
   </si>
   <si>
     <t>https://www.facebook.com/pstoyreviews</t>
@@ -6951,40 +7128,40 @@
         <v>595</v>
       </c>
       <c r="M5" t="s">
-        <v>600</v>
+        <v>610</v>
       </c>
       <c r="N5" t="s">
-        <v>605</v>
+        <v>625</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>617</v>
+        <v>640</v>
       </c>
       <c r="P5" t="s">
-        <v>627</v>
+        <v>650</v>
       </c>
       <c r="Q5" t="s">
-        <v>630</v>
+        <v>660</v>
       </c>
       <c r="R5" t="s">
-        <v>633</v>
+        <v>670</v>
       </c>
       <c r="T5">
         <v>150000</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>636</v>
+        <v>680</v>
       </c>
       <c r="W5" t="s">
-        <v>644</v>
+        <v>688</v>
       </c>
       <c r="X5" t="s">
-        <v>647</v>
+        <v>696</v>
       </c>
       <c r="Y5" t="s">
-        <v>650</v>
+        <v>701</v>
       </c>
       <c r="Z5" t="s">
-        <v>653</v>
+        <v>708</v>
       </c>
       <c r="AA5">
         <v>0</v>
@@ -7022,10 +7199,10 @@
         <v>596</v>
       </c>
       <c r="M6" t="s">
-        <v>601</v>
+        <v>611</v>
       </c>
       <c r="N6" t="s">
-        <v>606</v>
+        <v>626</v>
       </c>
     </row>
     <row r="7" spans="1:30">
@@ -7054,10 +7231,10 @@
         <v>597</v>
       </c>
       <c r="M7" t="s">
-        <v>602</v>
+        <v>612</v>
       </c>
       <c r="N7" t="s">
-        <v>607</v>
+        <v>627</v>
       </c>
     </row>
     <row r="8" spans="1:30">
@@ -7086,40 +7263,40 @@
         <v>598</v>
       </c>
       <c r="M8" t="s">
-        <v>603</v>
+        <v>613</v>
       </c>
       <c r="N8" t="s">
-        <v>608</v>
+        <v>628</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>618</v>
+        <v>641</v>
       </c>
       <c r="P8" t="s">
-        <v>628</v>
+        <v>651</v>
       </c>
       <c r="Q8" t="s">
-        <v>631</v>
+        <v>661</v>
       </c>
       <c r="R8" t="s">
-        <v>634</v>
+        <v>671</v>
       </c>
       <c r="T8">
         <v>600</v>
       </c>
       <c r="V8" s="2" t="s">
-        <v>637</v>
+        <v>681</v>
       </c>
       <c r="W8" t="s">
-        <v>645</v>
+        <v>689</v>
       </c>
       <c r="X8" t="s">
-        <v>648</v>
+        <v>609</v>
       </c>
       <c r="Y8" t="s">
-        <v>651</v>
+        <v>702</v>
       </c>
       <c r="Z8" t="s">
-        <v>654</v>
+        <v>709</v>
       </c>
       <c r="AA8">
         <v>1</v>
@@ -7128,7 +7305,7 @@
         <v>10</v>
       </c>
       <c r="AC8" s="2" t="s">
-        <v>656</v>
+        <v>715</v>
       </c>
       <c r="AD8">
         <v>5.962</v>
@@ -7160,40 +7337,40 @@
         <v>599</v>
       </c>
       <c r="M9" t="s">
-        <v>604</v>
+        <v>614</v>
       </c>
       <c r="N9" t="s">
-        <v>609</v>
+        <v>629</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>619</v>
+        <v>642</v>
       </c>
       <c r="P9" t="s">
-        <v>629</v>
+        <v>652</v>
       </c>
       <c r="Q9" t="s">
-        <v>632</v>
+        <v>662</v>
       </c>
       <c r="R9" t="s">
-        <v>635</v>
+        <v>672</v>
       </c>
       <c r="T9">
         <v>30</v>
       </c>
       <c r="V9" s="2" t="s">
-        <v>638</v>
+        <v>682</v>
       </c>
       <c r="W9" t="s">
-        <v>646</v>
+        <v>690</v>
       </c>
       <c r="X9" t="s">
-        <v>649</v>
+        <v>697</v>
       </c>
       <c r="Y9" t="s">
-        <v>652</v>
+        <v>703</v>
       </c>
       <c r="Z9" t="s">
-        <v>655</v>
+        <v>710</v>
       </c>
     </row>
     <row r="10" spans="1:30">
@@ -7221,29 +7398,32 @@
       <c r="K10" s="2" t="s">
         <v>585</v>
       </c>
-      <c r="L10">
-        <v>1.623</v>
-      </c>
-      <c r="M10">
-        <v>142000</v>
+      <c r="L10" t="s">
+        <v>600</v>
+      </c>
+      <c r="M10" t="s">
+        <v>615</v>
       </c>
       <c r="N10" t="s">
-        <v>610</v>
+        <v>630</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>620</v>
-      </c>
-      <c r="P10">
-        <v>1.018</v>
-      </c>
-      <c r="Q10">
-        <v>1.065</v>
-      </c>
-      <c r="R10">
-        <v>69</v>
+        <v>643</v>
+      </c>
+      <c r="P10" t="s">
+        <v>653</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>663</v>
+      </c>
+      <c r="R10" t="s">
+        <v>673</v>
       </c>
       <c r="V10" s="2" t="s">
-        <v>639</v>
+        <v>683</v>
+      </c>
+      <c r="W10" t="s">
+        <v>691</v>
       </c>
       <c r="AA10">
         <v>0</v>
@@ -7277,32 +7457,44 @@
       <c r="K11" s="2" t="s">
         <v>586</v>
       </c>
-      <c r="L11">
-        <v>1.118</v>
-      </c>
-      <c r="M11">
-        <v>96800</v>
+      <c r="L11" t="s">
+        <v>601</v>
+      </c>
+      <c r="M11" t="s">
+        <v>616</v>
       </c>
       <c r="N11" t="s">
-        <v>611</v>
+        <v>631</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>621</v>
-      </c>
-      <c r="P11">
-        <v>1.272</v>
-      </c>
-      <c r="Q11">
-        <v>2.309</v>
-      </c>
-      <c r="R11">
-        <v>5.554</v>
+        <v>644</v>
+      </c>
+      <c r="P11" t="s">
+        <v>654</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>664</v>
+      </c>
+      <c r="R11" t="s">
+        <v>674</v>
       </c>
       <c r="T11">
         <v>30</v>
       </c>
       <c r="V11" s="2" t="s">
-        <v>640</v>
+        <v>684</v>
+      </c>
+      <c r="W11" t="s">
+        <v>692</v>
+      </c>
+      <c r="X11" t="s">
+        <v>698</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>704</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>711</v>
       </c>
       <c r="AA11">
         <v>0</v>
@@ -7311,7 +7503,7 @@
         <v>0</v>
       </c>
       <c r="AC11" s="2" t="s">
-        <v>657</v>
+        <v>716</v>
       </c>
       <c r="AD11">
         <v>188</v>
@@ -7342,32 +7534,44 @@
       <c r="K12" s="2" t="s">
         <v>587</v>
       </c>
-      <c r="L12">
-        <v>1.224</v>
-      </c>
-      <c r="M12">
-        <v>53700</v>
+      <c r="L12" t="s">
+        <v>602</v>
+      </c>
+      <c r="M12" t="s">
+        <v>617</v>
       </c>
       <c r="N12" t="s">
-        <v>612</v>
+        <v>632</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>622</v>
-      </c>
-      <c r="P12">
-        <v>11</v>
-      </c>
-      <c r="Q12">
-        <v>132</v>
-      </c>
-      <c r="R12">
-        <v>2</v>
+        <v>645</v>
+      </c>
+      <c r="P12" t="s">
+        <v>655</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>665</v>
+      </c>
+      <c r="R12" t="s">
+        <v>675</v>
       </c>
       <c r="T12">
         <v>30</v>
       </c>
       <c r="V12" s="2" t="s">
-        <v>641</v>
+        <v>685</v>
+      </c>
+      <c r="W12" t="s">
+        <v>693</v>
+      </c>
+      <c r="X12" t="s">
+        <v>609</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>705</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>712</v>
       </c>
     </row>
     <row r="13" spans="1:30">
@@ -7392,32 +7596,44 @@
       <c r="K13" s="2" t="s">
         <v>588</v>
       </c>
-      <c r="L13">
-        <v>216</v>
-      </c>
-      <c r="M13">
-        <v>88600</v>
+      <c r="L13" t="s">
+        <v>603</v>
+      </c>
+      <c r="M13" t="s">
+        <v>618</v>
       </c>
       <c r="N13" t="s">
-        <v>613</v>
+        <v>633</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>623</v>
-      </c>
-      <c r="P13">
-        <v>270</v>
-      </c>
-      <c r="Q13">
-        <v>1.323</v>
-      </c>
-      <c r="R13">
-        <v>488</v>
+        <v>646</v>
+      </c>
+      <c r="P13" t="s">
+        <v>656</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>666</v>
+      </c>
+      <c r="R13" t="s">
+        <v>676</v>
       </c>
       <c r="T13">
         <v>50</v>
       </c>
       <c r="V13" s="2" t="s">
-        <v>642</v>
+        <v>686</v>
+      </c>
+      <c r="W13" t="s">
+        <v>694</v>
+      </c>
+      <c r="X13" t="s">
+        <v>699</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>706</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>713</v>
       </c>
       <c r="AA13">
         <v>1</v>
@@ -7426,7 +7642,7 @@
         <v>10</v>
       </c>
       <c r="AC13" s="2" t="s">
-        <v>658</v>
+        <v>717</v>
       </c>
       <c r="AD13">
         <v>236</v>
@@ -7451,14 +7667,14 @@
       <c r="K14" s="2" t="s">
         <v>589</v>
       </c>
-      <c r="L14">
-        <v>338</v>
-      </c>
-      <c r="M14">
-        <v>54800</v>
+      <c r="L14" t="s">
+        <v>604</v>
+      </c>
+      <c r="M14" t="s">
+        <v>619</v>
       </c>
       <c r="N14" t="s">
-        <v>614</v>
+        <v>634</v>
       </c>
     </row>
     <row r="15" spans="1:30">
@@ -7480,32 +7696,32 @@
       <c r="K15" s="2" t="s">
         <v>590</v>
       </c>
-      <c r="L15">
-        <v>536</v>
-      </c>
-      <c r="M15">
-        <v>42100</v>
+      <c r="L15" t="s">
+        <v>605</v>
+      </c>
+      <c r="M15" t="s">
+        <v>620</v>
       </c>
       <c r="N15" t="s">
-        <v>615</v>
+        <v>635</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>624</v>
-      </c>
-      <c r="P15">
-        <v>1.153</v>
-      </c>
-      <c r="Q15">
-        <v>1.113</v>
-      </c>
-      <c r="R15">
-        <v>391</v>
+        <v>647</v>
+      </c>
+      <c r="P15" t="s">
+        <v>657</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>667</v>
+      </c>
+      <c r="R15" t="s">
+        <v>677</v>
       </c>
       <c r="T15">
         <v>30</v>
       </c>
       <c r="AC15" s="2" t="s">
-        <v>659</v>
+        <v>718</v>
       </c>
       <c r="AD15">
         <v>57</v>
@@ -7533,47 +7749,47 @@
       <c r="K16" s="2" t="s">
         <v>591</v>
       </c>
-      <c r="L16">
-        <v>165</v>
-      </c>
-      <c r="M16">
-        <v>49600</v>
+      <c r="L16" t="s">
+        <v>606</v>
+      </c>
+      <c r="M16" t="s">
+        <v>621</v>
       </c>
       <c r="N16" t="s">
-        <v>616</v>
+        <v>636</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>625</v>
-      </c>
-      <c r="P16">
-        <v>260</v>
-      </c>
-      <c r="Q16">
-        <v>754</v>
-      </c>
-      <c r="R16">
-        <v>330</v>
+        <v>648</v>
+      </c>
+      <c r="P16" t="s">
+        <v>658</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>668</v>
+      </c>
+      <c r="R16" t="s">
+        <v>678</v>
       </c>
       <c r="T16">
         <v>100</v>
       </c>
       <c r="V16" s="2" t="s">
-        <v>643</v>
-      </c>
-      <c r="W16">
+        <v>687</v>
+      </c>
+      <c r="W16" t="s">
+        <v>695</v>
+      </c>
+      <c r="X16" t="s">
+        <v>700</v>
+      </c>
+      <c r="Y16" t="s">
         <v>707</v>
       </c>
-      <c r="X16">
-        <v>142</v>
-      </c>
-      <c r="Y16">
-        <v>547</v>
-      </c>
-      <c r="Z16">
-        <v>1.004</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15">
+      <c r="Z16" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -7589,8 +7805,17 @@
       <c r="K17" s="2" t="s">
         <v>592</v>
       </c>
-    </row>
-    <row r="18" spans="1:15">
+      <c r="L17" t="s">
+        <v>607</v>
+      </c>
+      <c r="M17" t="s">
+        <v>622</v>
+      </c>
+      <c r="N17" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -7600,8 +7825,17 @@
       <c r="K18" s="2" t="s">
         <v>593</v>
       </c>
-    </row>
-    <row r="19" spans="1:15">
+      <c r="L18" t="s">
+        <v>608</v>
+      </c>
+      <c r="M18" t="s">
+        <v>623</v>
+      </c>
+      <c r="N18" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -7611,8 +7845,17 @@
       <c r="K19" s="2" t="s">
         <v>594</v>
       </c>
-    </row>
-    <row r="20" spans="1:15">
+      <c r="L19" t="s">
+        <v>609</v>
+      </c>
+      <c r="M19" t="s">
+        <v>624</v>
+      </c>
+      <c r="N19" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -7620,7 +7863,16 @@
         <v>559</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>626</v>
+        <v>649</v>
+      </c>
+      <c r="P20" t="s">
+        <v>659</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>669</v>
+      </c>
+      <c r="R20" t="s">
+        <v>679</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed a bug in twitter funcs
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1132" uniqueCount="719">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1134" uniqueCount="721">
   <si>
     <t>Contact Name</t>
   </si>
@@ -1802,7 +1802,7 @@
     <t>https://www.youtube.com/channel/Japan</t>
   </si>
   <si>
-    <t>2239</t>
+    <t>2241</t>
   </si>
   <si>
     <t>2031</t>
@@ -1811,7 +1811,7 @@
     <t>1844</t>
   </si>
   <si>
-    <t>3869</t>
+    <t>3870</t>
   </si>
   <si>
     <t>101</t>
@@ -1820,16 +1820,16 @@
     <t>1623</t>
   </si>
   <si>
-    <t>1123</t>
-  </si>
-  <si>
-    <t>1228</t>
+    <t>1111</t>
+  </si>
+  <si>
+    <t>1229</t>
   </si>
   <si>
     <t>217</t>
   </si>
   <si>
-    <t>335</t>
+    <t>330</t>
   </si>
   <si>
     <t>537</t>
@@ -1868,10 +1868,10 @@
     <t>96.9K</t>
   </si>
   <si>
-    <t>53.9K</t>
-  </si>
-  <si>
-    <t>93K</t>
+    <t>54K</t>
+  </si>
+  <si>
+    <t>93.5K</t>
   </si>
   <si>
     <t>55K</t>
@@ -1880,10 +1880,10 @@
     <t>42.2K</t>
   </si>
   <si>
-    <t>50.8K</t>
-  </si>
-  <si>
-    <t>32.9K</t>
+    <t>51K</t>
+  </si>
+  <si>
+    <t>33.1K</t>
   </si>
   <si>
     <t>101M</t>
@@ -1892,49 +1892,49 @@
     <t>1.15K</t>
   </si>
   <si>
-    <t>3903113533</t>
-  </si>
-  <si>
-    <t>2552677239</t>
-  </si>
-  <si>
-    <t>1359421232</t>
-  </si>
-  <si>
-    <t>859283273</t>
-  </si>
-  <si>
-    <t>46542627</t>
-  </si>
-  <si>
-    <t>72626322</t>
-  </si>
-  <si>
-    <t>101237916</t>
-  </si>
-  <si>
-    <t>59753446</t>
-  </si>
-  <si>
-    <t>25555069</t>
-  </si>
-  <si>
-    <t>19657263</t>
-  </si>
-  <si>
-    <t>33873652</t>
-  </si>
-  <si>
-    <t>10271855</t>
-  </si>
-  <si>
-    <t>8866893</t>
-  </si>
-  <si>
-    <t>23474006016</t>
-  </si>
-  <si>
-    <t>330218</t>
+    <t>3904142596</t>
+  </si>
+  <si>
+    <t>2553803768</t>
+  </si>
+  <si>
+    <t>1359630995</t>
+  </si>
+  <si>
+    <t>859514058</t>
+  </si>
+  <si>
+    <t>46651885</t>
+  </si>
+  <si>
+    <t>72635441</t>
+  </si>
+  <si>
+    <t>101249439</t>
+  </si>
+  <si>
+    <t>59781475</t>
+  </si>
+  <si>
+    <t>25705893</t>
+  </si>
+  <si>
+    <t>19663349</t>
+  </si>
+  <si>
+    <t>33879805</t>
+  </si>
+  <si>
+    <t>10374071</t>
+  </si>
+  <si>
+    <t>8922883</t>
+  </si>
+  <si>
+    <t>23486563004</t>
+  </si>
+  <si>
+    <t>330219</t>
   </si>
   <si>
     <t>https://www.instagram.com/teamawesmr/</t>
@@ -1979,7 +1979,7 @@
     <t>1,018</t>
   </si>
   <si>
-    <t>1,278</t>
+    <t>1,279</t>
   </si>
   <si>
     <t>11</t>
@@ -2003,13 +2003,13 @@
     <t>27.2k</t>
   </si>
   <si>
-    <t>1,249</t>
+    <t>1,254</t>
   </si>
   <si>
     <t>1,066</t>
   </si>
   <si>
-    <t>2,332</t>
+    <t>2,334</t>
   </si>
   <si>
     <t>134</t>
@@ -2021,10 +2021,10 @@
     <t>1,114</t>
   </si>
   <si>
-    <t>762</t>
-  </si>
-  <si>
-    <t>154</t>
+    <t>765</t>
+  </si>
+  <si>
+    <t>153</t>
   </si>
   <si>
     <t>0</t>
@@ -2039,7 +2039,7 @@
     <t>69</t>
   </si>
   <si>
-    <t>5,780</t>
+    <t>5,777</t>
   </si>
   <si>
     <t>2</t>
@@ -2054,7 +2054,7 @@
     <t>333</t>
   </si>
   <si>
-    <t>200</t>
+    <t>161</t>
   </si>
   <si>
     <t>https://twitter.com/teamAWESMR</t>
@@ -2102,7 +2102,7 @@
     <t>796</t>
   </si>
   <si>
-    <t>706</t>
+    <t>708</t>
   </si>
   <si>
     <t>57</t>
@@ -2111,7 +2111,7 @@
     <t>727</t>
   </si>
   <si>
-    <t>1403</t>
+    <t>1402</t>
   </si>
   <si>
     <t>259</t>
@@ -2129,6 +2129,9 @@
     <t>1530</t>
   </si>
   <si>
+    <t>9</t>
+  </si>
+  <si>
     <t>33</t>
   </si>
   <si>
@@ -2148,6 +2151,9 @@
   </si>
   <si>
     <t>1130</t>
+  </si>
+  <si>
+    <t>47</t>
   </si>
   <si>
     <t>8328</t>
@@ -7161,7 +7167,7 @@
         <v>701</v>
       </c>
       <c r="Z5" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="AA5">
         <v>0</v>
@@ -7296,7 +7302,7 @@
         <v>702</v>
       </c>
       <c r="Z8" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="AA8">
         <v>1</v>
@@ -7305,7 +7311,7 @@
         <v>10</v>
       </c>
       <c r="AC8" s="2" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="AD8">
         <v>5.962</v>
@@ -7370,7 +7376,7 @@
         <v>703</v>
       </c>
       <c r="Z9" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
     </row>
     <row r="10" spans="1:30">
@@ -7425,6 +7431,12 @@
       <c r="W10" t="s">
         <v>691</v>
       </c>
+      <c r="Y10" t="s">
+        <v>704</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>712</v>
+      </c>
       <c r="AA10">
         <v>0</v>
       </c>
@@ -7491,10 +7503,10 @@
         <v>698</v>
       </c>
       <c r="Y11" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="Z11" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="AA11">
         <v>0</v>
@@ -7503,7 +7515,7 @@
         <v>0</v>
       </c>
       <c r="AC11" s="2" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="AD11">
         <v>188</v>
@@ -7568,10 +7580,10 @@
         <v>609</v>
       </c>
       <c r="Y12" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="Z12" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
     </row>
     <row r="13" spans="1:30">
@@ -7630,10 +7642,10 @@
         <v>699</v>
       </c>
       <c r="Y13" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="Z13" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="AA13">
         <v>1</v>
@@ -7642,7 +7654,7 @@
         <v>10</v>
       </c>
       <c r="AC13" s="2" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="AD13">
         <v>236</v>
@@ -7721,7 +7733,7 @@
         <v>30</v>
       </c>
       <c r="AC15" s="2" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="AD15">
         <v>57</v>
@@ -7783,10 +7795,10 @@
         <v>700</v>
       </c>
       <c r="Y16" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="Z16" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
     </row>
     <row r="17" spans="1:18">

</xml_diff>

<commit_message>
Configured the web driver not to load images
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1802,16 +1802,16 @@
     <t>https://www.youtube.com/channel/Japan</t>
   </si>
   <si>
-    <t>2241</t>
-  </si>
-  <si>
-    <t>2031</t>
+    <t>2242</t>
+  </si>
+  <si>
+    <t>2032</t>
   </si>
   <si>
     <t>1844</t>
   </si>
   <si>
-    <t>3870</t>
+    <t>3871</t>
   </si>
   <si>
     <t>101</t>
@@ -1820,7 +1820,7 @@
     <t>1623</t>
   </si>
   <si>
-    <t>1111</t>
+    <t>1091</t>
   </si>
   <si>
     <t>1229</t>
@@ -1832,13 +1832,13 @@
     <t>330</t>
   </si>
   <si>
-    <t>537</t>
+    <t>538</t>
   </si>
   <si>
     <t>166</t>
   </si>
   <si>
-    <t>23</t>
+    <t>24</t>
   </si>
   <si>
     <t>3958</t>
@@ -1850,7 +1850,7 @@
     <t>5.62M</t>
   </si>
   <si>
-    <t>2.46M</t>
+    <t>2.47M</t>
   </si>
   <si>
     <t>1.78M</t>
@@ -1859,7 +1859,7 @@
     <t>1.46M</t>
   </si>
   <si>
-    <t>253K</t>
+    <t>254K</t>
   </si>
   <si>
     <t>143K</t>
@@ -1871,7 +1871,7 @@
     <t>54K</t>
   </si>
   <si>
-    <t>93.5K</t>
+    <t>94.2K</t>
   </si>
   <si>
     <t>55K</t>
@@ -1880,10 +1880,10 @@
     <t>42.2K</t>
   </si>
   <si>
-    <t>51K</t>
-  </si>
-  <si>
-    <t>33.1K</t>
+    <t>51.3K</t>
+  </si>
+  <si>
+    <t>33.2K</t>
   </si>
   <si>
     <t>101M</t>
@@ -1892,49 +1892,49 @@
     <t>1.15K</t>
   </si>
   <si>
-    <t>3904142596</t>
-  </si>
-  <si>
-    <t>2553803768</t>
-  </si>
-  <si>
-    <t>1359630995</t>
-  </si>
-  <si>
-    <t>859514058</t>
-  </si>
-  <si>
-    <t>46651885</t>
-  </si>
-  <si>
-    <t>72635441</t>
-  </si>
-  <si>
-    <t>101249439</t>
-  </si>
-  <si>
-    <t>59781475</t>
-  </si>
-  <si>
-    <t>25705893</t>
-  </si>
-  <si>
-    <t>19663349</t>
-  </si>
-  <si>
-    <t>33879805</t>
-  </si>
-  <si>
-    <t>10374071</t>
-  </si>
-  <si>
-    <t>8922883</t>
-  </si>
-  <si>
-    <t>23486563004</t>
-  </si>
-  <si>
-    <t>330219</t>
+    <t>3905158114</t>
+  </si>
+  <si>
+    <t>2554596251</t>
+  </si>
+  <si>
+    <t>1359840147</t>
+  </si>
+  <si>
+    <t>859757527</t>
+  </si>
+  <si>
+    <t>46756400</t>
+  </si>
+  <si>
+    <t>72643506</t>
+  </si>
+  <si>
+    <t>101262763</t>
+  </si>
+  <si>
+    <t>59807827</t>
+  </si>
+  <si>
+    <t>25914850</t>
+  </si>
+  <si>
+    <t>19574471</t>
+  </si>
+  <si>
+    <t>33887803</t>
+  </si>
+  <si>
+    <t>10483531</t>
+  </si>
+  <si>
+    <t>8974378</t>
+  </si>
+  <si>
+    <t>23496457944</t>
+  </si>
+  <si>
+    <t>330221</t>
   </si>
   <si>
     <t>https://www.instagram.com/teamawesmr/</t>
@@ -1967,7 +1967,7 @@
     <t>https://www.instagram.com/hazarblablabla/</t>
   </si>
   <si>
-    <t>114</t>
+    <t>115</t>
   </si>
   <si>
     <t>289</t>
@@ -1979,28 +1979,28 @@
     <t>1,018</t>
   </si>
   <si>
-    <t>1,279</t>
+    <t>1,280</t>
   </si>
   <si>
     <t>11</t>
   </si>
   <si>
-    <t>275</t>
+    <t>276</t>
   </si>
   <si>
     <t>1,153</t>
   </si>
   <si>
-    <t>265</t>
+    <t>266</t>
   </si>
   <si>
     <t>17</t>
   </si>
   <si>
-    <t>42.6k</t>
-  </si>
-  <si>
-    <t>27.2k</t>
+    <t>42.7k</t>
+  </si>
+  <si>
+    <t>27.3k</t>
   </si>
   <si>
     <t>1,254</t>
@@ -2009,16 +2009,16 @@
     <t>1,066</t>
   </si>
   <si>
-    <t>2,334</t>
+    <t>2,336</t>
   </si>
   <si>
     <t>134</t>
   </si>
   <si>
-    <t>1,323</t>
-  </si>
-  <si>
-    <t>1,114</t>
+    <t>1,325</t>
+  </si>
+  <si>
+    <t>1,112</t>
   </si>
   <si>
     <t>765</t>
@@ -2033,13 +2033,13 @@
     <t>38</t>
   </si>
   <si>
-    <t>2,325</t>
+    <t>2,324</t>
   </si>
   <si>
     <t>69</t>
   </si>
   <si>
-    <t>5,777</t>
+    <t>5,776</t>
   </si>
   <si>
     <t>2</t>
@@ -2087,7 +2087,7 @@
     <t>1963</t>
   </si>
   <si>
-    <t>960</t>
+    <t>961</t>
   </si>
   <si>
     <t>5</t>
@@ -2099,7 +2099,7 @@
     <t>44</t>
   </si>
   <si>
-    <t>796</t>
+    <t>794</t>
   </si>
   <si>
     <t>708</t>

</xml_diff>

<commit_message>
Driver stops loading when it finds the element wanted. Decreased the total execution time tremendously
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1814,7 +1814,7 @@
     <t>3871</t>
   </si>
   <si>
-    <t>101</t>
+    <t>102</t>
   </si>
   <si>
     <t>1623</t>
@@ -1841,7 +1841,7 @@
     <t>24</t>
   </si>
   <si>
-    <t>3958</t>
+    <t>3959</t>
   </si>
   <si>
     <t>16</t>
@@ -1892,22 +1892,22 @@
     <t>1.15K</t>
   </si>
   <si>
-    <t>3905158114</t>
+    <t>3905221144</t>
   </si>
   <si>
     <t>2554596251</t>
   </si>
   <si>
-    <t>1359840147</t>
-  </si>
-  <si>
-    <t>859757527</t>
-  </si>
-  <si>
-    <t>46756400</t>
-  </si>
-  <si>
-    <t>72643506</t>
+    <t>1359866729</t>
+  </si>
+  <si>
+    <t>859772858</t>
+  </si>
+  <si>
+    <t>46813319</t>
+  </si>
+  <si>
+    <t>72644659</t>
   </si>
   <si>
     <t>101262763</t>
@@ -1919,7 +1919,7 @@
     <t>25914850</t>
   </si>
   <si>
-    <t>19574471</t>
+    <t>19575222</t>
   </si>
   <si>
     <t>33887803</t>
@@ -1931,7 +1931,7 @@
     <t>8974378</t>
   </si>
   <si>
-    <t>23496457944</t>
+    <t>23496930482</t>
   </si>
   <si>
     <t>330221</t>
@@ -2099,7 +2099,7 @@
     <t>44</t>
   </si>
   <si>
-    <t>794</t>
+    <t>795</t>
   </si>
   <si>
     <t>708</t>
@@ -2126,7 +2126,7 @@
     <t>12</t>
   </si>
   <si>
-    <t>1530</t>
+    <t>1531</t>
   </si>
   <si>
     <t>9</t>
@@ -2159,7 +2159,7 @@
     <t>8328</t>
   </si>
   <si>
-    <t>775</t>
+    <t>776</t>
   </si>
   <si>
     <t>282</t>

</xml_diff>

<commit_message>
Instagram function uses a profile to avoid getting band.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2154" uniqueCount="1199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2196" uniqueCount="1240">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -3147,10 +3147,10 @@
     <t>1866</t>
   </si>
   <si>
-    <t>3920</t>
-  </si>
-  <si>
-    <t>111</t>
+    <t>3921</t>
+  </si>
+  <si>
+    <t>112</t>
   </si>
   <si>
     <t>1623</t>
@@ -3162,7 +3162,7 @@
     <t>1256</t>
   </si>
   <si>
-    <t>226</t>
+    <t>227</t>
   </si>
   <si>
     <t>284</t>
@@ -3177,7 +3177,40 @@
     <t>33</t>
   </si>
   <si>
-    <t>5.76M</t>
+    <t>120</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>2545</t>
+  </si>
+  <si>
+    <t>472</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>160</t>
+  </si>
+  <si>
+    <t>530</t>
+  </si>
+  <si>
+    <t>412</t>
+  </si>
+  <si>
+    <t>172</t>
+  </si>
+  <si>
+    <t>560</t>
+  </si>
+  <si>
+    <t>488</t>
+  </si>
+  <si>
+    <t>5.77M</t>
   </si>
   <si>
     <t>2.53M</t>
@@ -3189,7 +3222,7 @@
     <t>1.48M</t>
   </si>
   <si>
-    <t>370K</t>
+    <t>373K</t>
   </si>
   <si>
     <t>144K</t>
@@ -3201,91 +3234,121 @@
     <t>55.4K</t>
   </si>
   <si>
-    <t>123K</t>
+    <t>124K</t>
   </si>
   <si>
     <t>56.4K</t>
   </si>
   <si>
-    <t>43K</t>
-  </si>
-  <si>
-    <t>92.3K</t>
-  </si>
-  <si>
-    <t>66.4K</t>
-  </si>
-  <si>
-    <t>11.8K</t>
-  </si>
-  <si>
-    <t>239K</t>
-  </si>
-  <si>
-    <t>13.7M</t>
-  </si>
-  <si>
-    <t>685K</t>
-  </si>
-  <si>
-    <t>6.71K</t>
-  </si>
-  <si>
-    <t>5.4M</t>
-  </si>
-  <si>
-    <t>6M</t>
-  </si>
-  <si>
-    <t>34.3K</t>
-  </si>
-  <si>
-    <t>88K</t>
-  </si>
-  <si>
-    <t>156K</t>
-  </si>
-  <si>
-    <t>11.9M</t>
-  </si>
-  <si>
-    <t>3978532128</t>
-  </si>
-  <si>
-    <t>2581556080</t>
-  </si>
-  <si>
-    <t>1379016605</t>
-  </si>
-  <si>
-    <t>874270969</t>
-  </si>
-  <si>
-    <t>67928960</t>
-  </si>
-  <si>
-    <t>73262104</t>
-  </si>
-  <si>
-    <t>102916385</t>
-  </si>
-  <si>
-    <t>61291865</t>
-  </si>
-  <si>
-    <t>35590495</t>
-  </si>
-  <si>
-    <t>16958227</t>
-  </si>
-  <si>
-    <t>34535260</t>
-  </si>
-  <si>
-    <t>22323588</t>
-  </si>
-  <si>
-    <t>19244603</t>
+    <t>43.1K</t>
+  </si>
+  <si>
+    <t>93.5K</t>
+  </si>
+  <si>
+    <t>69.4K</t>
+  </si>
+  <si>
+    <t>12K</t>
+  </si>
+  <si>
+    <t>246K</t>
+  </si>
+  <si>
+    <t>14.1M</t>
+  </si>
+  <si>
+    <t>835K</t>
+  </si>
+  <si>
+    <t>6.94K</t>
+  </si>
+  <si>
+    <t>6.3M</t>
+  </si>
+  <si>
+    <t>6.48M</t>
+  </si>
+  <si>
+    <t>92.2K</t>
+  </si>
+  <si>
+    <t>167K</t>
+  </si>
+  <si>
+    <t>12.7M</t>
+  </si>
+  <si>
+    <t>3980867842</t>
+  </si>
+  <si>
+    <t>2582359283</t>
+  </si>
+  <si>
+    <t>1379511884</t>
+  </si>
+  <si>
+    <t>874662593</t>
+  </si>
+  <si>
+    <t>68691343</t>
+  </si>
+  <si>
+    <t>73279057</t>
+  </si>
+  <si>
+    <t>102958564</t>
+  </si>
+  <si>
+    <t>61319131</t>
+  </si>
+  <si>
+    <t>35875442</t>
+  </si>
+  <si>
+    <t>16963924</t>
+  </si>
+  <si>
+    <t>34556510</t>
+  </si>
+  <si>
+    <t>22721523</t>
+  </si>
+  <si>
+    <t>20088488</t>
+  </si>
+  <si>
+    <t>523597</t>
+  </si>
+  <si>
+    <t>10186655</t>
+  </si>
+  <si>
+    <t>5749403195</t>
+  </si>
+  <si>
+    <t>669008754</t>
+  </si>
+  <si>
+    <t>1828962</t>
+  </si>
+  <si>
+    <t>4472336318</t>
+  </si>
+  <si>
+    <t>4558384287</t>
+  </si>
+  <si>
+    <t>2873831</t>
+  </si>
+  <si>
+    <t>6891161</t>
+  </si>
+  <si>
+    <t>40254561</t>
+  </si>
+  <si>
+    <t>5501391400</t>
   </si>
   <si>
     <t>https://www.instagram.com/teamawesmr/</t>
@@ -3330,28 +3393,28 @@
     <t>https://www.instagram.com/techsith/</t>
   </si>
   <si>
-    <t>144</t>
+    <t>145</t>
   </si>
   <si>
     <t>289</t>
   </si>
   <si>
-    <t>89</t>
+    <t>90</t>
   </si>
   <si>
     <t>1,018</t>
   </si>
   <si>
-    <t>1,382</t>
+    <t>1,383</t>
   </si>
   <si>
     <t>12</t>
   </si>
   <si>
-    <t>285</t>
-  </si>
-  <si>
-    <t>1,174</t>
+    <t>287</t>
+  </si>
+  <si>
+    <t>1,175</t>
   </si>
   <si>
     <t>297</t>
@@ -3363,70 +3426,70 @@
     <t>0</t>
   </si>
   <si>
-    <t>453</t>
+    <t>461</t>
   </si>
   <si>
     <t>387</t>
   </si>
   <si>
+    <t>121</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>49.5k</t>
+  </si>
+  <si>
+    <t>27.4k</t>
+  </si>
+  <si>
+    <t>1,277</t>
+  </si>
+  <si>
+    <t>1,063</t>
+  </si>
+  <si>
+    <t>2,403</t>
+  </si>
+  <si>
+    <t>1,332</t>
+  </si>
+  <si>
+    <t>1,110</t>
+  </si>
+  <si>
+    <t>808</t>
+  </si>
+  <si>
+    <t>684</t>
+  </si>
+  <si>
+    <t>32.1k</t>
+  </si>
+  <si>
+    <t>31.4k</t>
+  </si>
+  <si>
+    <t>4,789</t>
+  </si>
+  <si>
+    <t>217</t>
+  </si>
+  <si>
+    <t>113</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>2,341</t>
+  </si>
+  <si>
     <t>69</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>49.5k</t>
-  </si>
-  <si>
-    <t>27.4k</t>
-  </si>
-  <si>
-    <t>1,276</t>
-  </si>
-  <si>
-    <t>1,063</t>
-  </si>
-  <si>
-    <t>2,403</t>
-  </si>
-  <si>
-    <t>145</t>
-  </si>
-  <si>
-    <t>1,332</t>
-  </si>
-  <si>
-    <t>1,112</t>
-  </si>
-  <si>
-    <t>806</t>
-  </si>
-  <si>
-    <t>682</t>
-  </si>
-  <si>
-    <t>32.9k</t>
-  </si>
-  <si>
-    <t>30k</t>
-  </si>
-  <si>
-    <t>4,768</t>
-  </si>
-  <si>
-    <t>156</t>
-  </si>
-  <si>
-    <t>116</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>2,341</t>
-  </si>
-  <si>
-    <t>5,994</t>
+    <t>5,993</t>
   </si>
   <si>
     <t>2</t>
@@ -3444,13 +3507,13 @@
     <t>504</t>
   </si>
   <si>
-    <t>1,217</t>
-  </si>
-  <si>
-    <t>4,315</t>
-  </si>
-  <si>
-    <t>64</t>
+    <t>1,334</t>
+  </si>
+  <si>
+    <t>4,292</t>
+  </si>
+  <si>
+    <t>72</t>
   </si>
   <si>
     <t>5</t>
@@ -3498,34 +3561,49 @@
     <t>https://twitter.com/techsith1</t>
   </si>
   <si>
-    <t>1056</t>
-  </si>
-  <si>
-    <t>1981</t>
-  </si>
-  <si>
-    <t>977</t>
-  </si>
-  <si>
-    <t>659</t>
+    <t>1055</t>
+  </si>
+  <si>
+    <t>1982</t>
+  </si>
+  <si>
+    <t>978</t>
+  </si>
+  <si>
+    <t>658</t>
   </si>
   <si>
     <t>44</t>
   </si>
   <si>
-    <t>795</t>
+    <t>780</t>
   </si>
   <si>
     <t>723</t>
   </si>
   <si>
+    <t>3174</t>
+  </si>
+  <si>
+    <t>20582</t>
+  </si>
+  <si>
+    <t>17137</t>
+  </si>
+  <si>
+    <t>2215</t>
+  </si>
+  <si>
+    <t>1047</t>
+  </si>
+  <si>
     <t>57</t>
   </si>
   <si>
     <t>16</t>
   </si>
   <si>
-    <t>730</t>
+    <t>732</t>
   </si>
   <si>
     <t>1402</t>
@@ -3540,10 +3618,25 @@
     <t>8</t>
   </si>
   <si>
+    <t>747</t>
+  </si>
+  <si>
+    <t>821</t>
+  </si>
+  <si>
+    <t>630</t>
+  </si>
+  <si>
+    <t>869</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
     <t>10</t>
   </si>
   <si>
-    <t>1549</t>
+    <t>1550</t>
   </si>
   <si>
     <t>9</t>
@@ -3558,13 +3651,28 @@
     <t>554</t>
   </si>
   <si>
+    <t>2182</t>
+  </si>
+  <si>
+    <t>14020</t>
+  </si>
+  <si>
+    <t>9777</t>
+  </si>
+  <si>
+    <t>1126</t>
+  </si>
+  <si>
+    <t>159</t>
+  </si>
+  <si>
     <t>2049</t>
   </si>
   <si>
     <t>4136</t>
   </si>
   <si>
-    <t>1141</t>
+    <t>1144</t>
   </si>
   <si>
     <t>47</t>
@@ -3576,13 +3684,28 @@
     <t>802</t>
   </si>
   <si>
-    <t>280</t>
+    <t>281</t>
   </si>
   <si>
     <t>1027</t>
   </si>
   <si>
     <t>15</t>
+  </si>
+  <si>
+    <t>5245</t>
+  </si>
+  <si>
+    <t>2001</t>
+  </si>
+  <si>
+    <t>4917</t>
+  </si>
+  <si>
+    <t>3114</t>
+  </si>
+  <si>
+    <t>437</t>
   </si>
   <si>
     <t>https://www.facebook.com/pstoyreviews</t>
@@ -11175,40 +11298,40 @@
         <v>1038</v>
       </c>
       <c r="N5" t="s">
-        <v>1051</v>
+        <v>1062</v>
       </c>
       <c r="O5" t="s">
-        <v>1075</v>
+        <v>1085</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>1088</v>
+        <v>1109</v>
       </c>
       <c r="Q5" t="s">
-        <v>1102</v>
+        <v>1123</v>
       </c>
       <c r="R5" t="s">
-        <v>1117</v>
+        <v>1138</v>
       </c>
       <c r="S5" t="s">
-        <v>1112</v>
+        <v>1133</v>
       </c>
       <c r="U5">
         <v>150000</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>1144</v>
+        <v>1165</v>
       </c>
       <c r="X5" t="s">
-        <v>1158</v>
+        <v>1179</v>
       </c>
       <c r="Y5" t="s">
-        <v>1165</v>
+        <v>1191</v>
       </c>
       <c r="Z5" t="s">
-        <v>1172</v>
+        <v>1203</v>
       </c>
       <c r="AA5" t="s">
-        <v>1178</v>
+        <v>1214</v>
       </c>
       <c r="AB5">
         <v>0</v>
@@ -11246,10 +11369,10 @@
         <v>1039</v>
       </c>
       <c r="N6" t="s">
-        <v>1052</v>
+        <v>1063</v>
       </c>
       <c r="O6" t="s">
-        <v>1076</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="7" spans="1:31">
@@ -11275,10 +11398,10 @@
         <v>1040</v>
       </c>
       <c r="N7" t="s">
-        <v>1053</v>
+        <v>1064</v>
       </c>
       <c r="O7" t="s">
-        <v>1077</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="8" spans="1:31">
@@ -11304,40 +11427,40 @@
         <v>1041</v>
       </c>
       <c r="N8" t="s">
-        <v>1054</v>
+        <v>1065</v>
       </c>
       <c r="O8" t="s">
-        <v>1078</v>
+        <v>1088</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>1089</v>
+        <v>1110</v>
       </c>
       <c r="Q8" t="s">
-        <v>1103</v>
+        <v>1124</v>
       </c>
       <c r="R8" t="s">
-        <v>1118</v>
+        <v>1139</v>
       </c>
       <c r="S8" t="s">
-        <v>1132</v>
+        <v>1152</v>
       </c>
       <c r="U8">
         <v>600</v>
       </c>
       <c r="W8" s="2" t="s">
-        <v>1145</v>
+        <v>1166</v>
       </c>
       <c r="X8" t="s">
-        <v>1159</v>
+        <v>1180</v>
       </c>
       <c r="Y8" t="s">
-        <v>1166</v>
+        <v>1192</v>
       </c>
       <c r="Z8" t="s">
-        <v>1107</v>
+        <v>1128</v>
       </c>
       <c r="AA8" t="s">
-        <v>1179</v>
+        <v>1215</v>
       </c>
       <c r="AB8">
         <v>1</v>
@@ -11346,7 +11469,7 @@
         <v>10</v>
       </c>
       <c r="AD8" s="2" t="s">
-        <v>1187</v>
+        <v>1228</v>
       </c>
       <c r="AE8">
         <v>5962</v>
@@ -11378,40 +11501,40 @@
         <v>1042</v>
       </c>
       <c r="N9" t="s">
-        <v>1055</v>
+        <v>1066</v>
       </c>
       <c r="O9" t="s">
-        <v>1079</v>
+        <v>1089</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>1090</v>
+        <v>1111</v>
       </c>
       <c r="Q9" t="s">
-        <v>1104</v>
+        <v>1125</v>
       </c>
       <c r="R9" t="s">
-        <v>1119</v>
+        <v>1140</v>
       </c>
       <c r="S9" t="s">
-        <v>1133</v>
+        <v>1153</v>
       </c>
       <c r="U9">
         <v>30</v>
       </c>
       <c r="W9" s="2" t="s">
-        <v>1146</v>
+        <v>1167</v>
       </c>
       <c r="X9" t="s">
-        <v>1160</v>
+        <v>1181</v>
       </c>
       <c r="Y9" t="s">
-        <v>1167</v>
+        <v>1193</v>
       </c>
       <c r="Z9" t="s">
-        <v>1173</v>
+        <v>1204</v>
       </c>
       <c r="AA9" t="s">
-        <v>1180</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="10" spans="1:31">
@@ -11443,37 +11566,37 @@
         <v>1043</v>
       </c>
       <c r="N10" t="s">
-        <v>1056</v>
+        <v>1067</v>
       </c>
       <c r="O10" t="s">
-        <v>1080</v>
+        <v>1090</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>1091</v>
+        <v>1112</v>
       </c>
       <c r="Q10" t="s">
-        <v>1105</v>
+        <v>1126</v>
       </c>
       <c r="R10" t="s">
-        <v>1120</v>
+        <v>1141</v>
       </c>
       <c r="S10" t="s">
-        <v>1115</v>
+        <v>1154</v>
       </c>
       <c r="W10" s="2" t="s">
-        <v>1147</v>
+        <v>1168</v>
       </c>
       <c r="X10" t="s">
-        <v>1143</v>
+        <v>1164</v>
       </c>
       <c r="Y10">
         <v>84</v>
       </c>
       <c r="Z10" t="s">
-        <v>1174</v>
+        <v>1205</v>
       </c>
       <c r="AA10" t="s">
-        <v>1181</v>
+        <v>1217</v>
       </c>
       <c r="AB10">
         <v>0</v>
@@ -11511,40 +11634,40 @@
         <v>1044</v>
       </c>
       <c r="N11" t="s">
-        <v>1057</v>
+        <v>1068</v>
       </c>
       <c r="O11" t="s">
-        <v>1081</v>
+        <v>1091</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>1092</v>
+        <v>1113</v>
       </c>
       <c r="Q11" t="s">
-        <v>1106</v>
+        <v>1127</v>
       </c>
       <c r="R11" t="s">
-        <v>1121</v>
+        <v>1142</v>
       </c>
       <c r="S11" t="s">
-        <v>1134</v>
+        <v>1155</v>
       </c>
       <c r="U11">
         <v>30</v>
       </c>
       <c r="W11" s="2" t="s">
-        <v>1148</v>
+        <v>1169</v>
       </c>
       <c r="X11" t="s">
-        <v>1161</v>
+        <v>1182</v>
       </c>
       <c r="Y11" t="s">
-        <v>1168</v>
+        <v>1194</v>
       </c>
       <c r="Z11" t="s">
         <v>1050</v>
       </c>
       <c r="AA11" t="s">
-        <v>1182</v>
+        <v>1218</v>
       </c>
       <c r="AB11">
         <v>0</v>
@@ -11553,7 +11676,7 @@
         <v>0</v>
       </c>
       <c r="AD11" s="2" t="s">
-        <v>1188</v>
+        <v>1229</v>
       </c>
       <c r="AE11">
         <v>188</v>
@@ -11588,40 +11711,40 @@
         <v>1045</v>
       </c>
       <c r="N12" t="s">
-        <v>1058</v>
+        <v>1069</v>
       </c>
       <c r="O12" t="s">
-        <v>1082</v>
+        <v>1092</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>1093</v>
+        <v>1114</v>
       </c>
       <c r="Q12" t="s">
-        <v>1107</v>
+        <v>1128</v>
       </c>
       <c r="R12" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="S12" t="s">
-        <v>1135</v>
+        <v>1156</v>
       </c>
       <c r="U12">
         <v>30</v>
       </c>
       <c r="W12" s="2" t="s">
-        <v>1149</v>
+        <v>1170</v>
       </c>
       <c r="X12" t="s">
-        <v>1162</v>
+        <v>1183</v>
       </c>
       <c r="Y12" t="s">
-        <v>1166</v>
+        <v>1192</v>
       </c>
       <c r="Z12" t="s">
-        <v>1175</v>
+        <v>1206</v>
       </c>
       <c r="AA12" t="s">
-        <v>1183</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="13" spans="1:31">
@@ -11650,40 +11773,40 @@
         <v>1046</v>
       </c>
       <c r="N13" t="s">
-        <v>1059</v>
+        <v>1070</v>
       </c>
       <c r="O13" t="s">
-        <v>1083</v>
+        <v>1093</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>1094</v>
+        <v>1115</v>
       </c>
       <c r="Q13" t="s">
-        <v>1108</v>
+        <v>1129</v>
       </c>
       <c r="R13" t="s">
-        <v>1123</v>
+        <v>1143</v>
       </c>
       <c r="S13" t="s">
-        <v>1136</v>
+        <v>1157</v>
       </c>
       <c r="U13">
         <v>50</v>
       </c>
       <c r="W13" s="2" t="s">
-        <v>1150</v>
+        <v>1171</v>
       </c>
       <c r="X13" t="s">
-        <v>1163</v>
+        <v>1184</v>
       </c>
       <c r="Y13" t="s">
-        <v>1169</v>
+        <v>1195</v>
       </c>
       <c r="Z13" t="s">
-        <v>1176</v>
+        <v>1207</v>
       </c>
       <c r="AA13" t="s">
-        <v>1184</v>
+        <v>1220</v>
       </c>
       <c r="AB13">
         <v>1</v>
@@ -11692,7 +11815,7 @@
         <v>10</v>
       </c>
       <c r="AD13" s="2" t="s">
-        <v>1189</v>
+        <v>1230</v>
       </c>
       <c r="AE13">
         <v>236</v>
@@ -11724,10 +11847,10 @@
         <v>1047</v>
       </c>
       <c r="N14" t="s">
-        <v>1060</v>
+        <v>1071</v>
       </c>
       <c r="O14" t="s">
-        <v>1084</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="15" spans="1:31">
@@ -11756,28 +11879,28 @@
         <v>1048</v>
       </c>
       <c r="N15" t="s">
-        <v>1061</v>
+        <v>1072</v>
       </c>
       <c r="O15" t="s">
-        <v>1085</v>
+        <v>1095</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>1095</v>
+        <v>1116</v>
       </c>
       <c r="Q15" t="s">
-        <v>1109</v>
+        <v>1130</v>
       </c>
       <c r="R15" t="s">
-        <v>1124</v>
+        <v>1144</v>
       </c>
       <c r="S15" t="s">
-        <v>1137</v>
+        <v>1158</v>
       </c>
       <c r="U15">
         <v>30</v>
       </c>
       <c r="AD15" s="2" t="s">
-        <v>1190</v>
+        <v>1231</v>
       </c>
       <c r="AE15">
         <v>57</v>
@@ -11812,40 +11935,40 @@
         <v>1049</v>
       </c>
       <c r="N16" t="s">
-        <v>1062</v>
+        <v>1073</v>
       </c>
       <c r="O16" t="s">
-        <v>1086</v>
+        <v>1096</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>1096</v>
+        <v>1117</v>
       </c>
       <c r="Q16" t="s">
-        <v>1110</v>
+        <v>1131</v>
       </c>
       <c r="R16" t="s">
-        <v>1125</v>
+        <v>1145</v>
       </c>
       <c r="S16" t="s">
-        <v>1138</v>
+        <v>1159</v>
       </c>
       <c r="U16">
         <v>100</v>
       </c>
       <c r="W16" s="2" t="s">
-        <v>1151</v>
+        <v>1172</v>
       </c>
       <c r="X16" t="s">
-        <v>1164</v>
+        <v>1185</v>
       </c>
       <c r="Y16" t="s">
-        <v>1170</v>
+        <v>1196</v>
       </c>
       <c r="Z16" t="s">
-        <v>1177</v>
+        <v>1208</v>
       </c>
       <c r="AA16" t="s">
-        <v>1185</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="17" spans="1:31">
@@ -11874,37 +11997,37 @@
         <v>1050</v>
       </c>
       <c r="N17" t="s">
-        <v>1063</v>
+        <v>1074</v>
       </c>
       <c r="O17" t="s">
-        <v>1087</v>
+        <v>1097</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>1097</v>
+        <v>1118</v>
       </c>
       <c r="Q17" t="s">
-        <v>1111</v>
+        <v>1132</v>
       </c>
       <c r="R17" t="s">
-        <v>1126</v>
+        <v>1146</v>
       </c>
       <c r="S17" t="s">
-        <v>1139</v>
+        <v>1160</v>
       </c>
       <c r="U17">
         <v>30</v>
       </c>
       <c r="W17" s="2" t="s">
-        <v>1152</v>
+        <v>1173</v>
       </c>
       <c r="X17">
         <v>2</v>
       </c>
       <c r="Y17" t="s">
-        <v>1171</v>
+        <v>1197</v>
       </c>
       <c r="AA17" t="s">
-        <v>1186</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="18" spans="1:31">
@@ -11935,47 +12058,47 @@
       <c r="L18" s="2" t="s">
         <v>1027</v>
       </c>
-      <c r="M18">
-        <v>125</v>
+      <c r="M18" t="s">
+        <v>1051</v>
       </c>
       <c r="N18" t="s">
-        <v>1064</v>
-      </c>
-      <c r="O18">
-        <v>511507</v>
+        <v>1075</v>
+      </c>
+      <c r="O18" t="s">
+        <v>1098</v>
       </c>
       <c r="P18" s="2" t="s">
         <v>1027</v>
       </c>
       <c r="Q18" t="s">
-        <v>1112</v>
+        <v>1133</v>
       </c>
       <c r="R18" t="s">
-        <v>1127</v>
+        <v>1147</v>
       </c>
       <c r="S18" t="s">
-        <v>1112</v>
+        <v>1133</v>
       </c>
       <c r="U18">
         <v>600</v>
       </c>
       <c r="W18" s="2" t="s">
-        <v>1153</v>
-      </c>
-      <c r="X18">
-        <v>3127</v>
-      </c>
-      <c r="Y18">
-        <v>732</v>
-      </c>
-      <c r="Z18">
-        <v>2141</v>
-      </c>
-      <c r="AA18">
-        <v>5185</v>
+        <v>1174</v>
+      </c>
+      <c r="X18" t="s">
+        <v>1186</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>1198</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>1209</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>1223</v>
       </c>
       <c r="AD18" s="2" t="s">
-        <v>1191</v>
+        <v>1232</v>
       </c>
       <c r="AE18" s="3">
         <v>43467</v>
@@ -12006,44 +12129,44 @@
       <c r="L19" s="2" t="s">
         <v>1028</v>
       </c>
-      <c r="M19">
-        <v>68</v>
+      <c r="M19" t="s">
+        <v>1052</v>
       </c>
       <c r="N19" t="s">
-        <v>1065</v>
-      </c>
-      <c r="O19">
-        <v>9777119</v>
+        <v>1076</v>
+      </c>
+      <c r="O19" t="s">
+        <v>1099</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>1098</v>
+        <v>1119</v>
       </c>
       <c r="Q19" t="s">
-        <v>1113</v>
+        <v>1134</v>
       </c>
       <c r="R19" t="s">
-        <v>1128</v>
+        <v>1148</v>
       </c>
       <c r="S19" t="s">
-        <v>1140</v>
+        <v>1161</v>
       </c>
       <c r="U19">
         <v>2000</v>
       </c>
       <c r="W19" s="2" t="s">
-        <v>1154</v>
-      </c>
-      <c r="X19">
-        <v>19300</v>
-      </c>
-      <c r="Y19">
-        <v>776</v>
-      </c>
-      <c r="Z19">
-        <v>13510</v>
-      </c>
-      <c r="AA19">
-        <v>1945</v>
+        <v>1175</v>
+      </c>
+      <c r="X19" t="s">
+        <v>1187</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>1199</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>1210</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>1224</v>
       </c>
     </row>
     <row r="20" spans="1:31">
@@ -12074,29 +12197,29 @@
       <c r="L20" s="2" t="s">
         <v>1029</v>
       </c>
-      <c r="M20">
-        <v>2495</v>
+      <c r="M20" t="s">
+        <v>1053</v>
       </c>
       <c r="N20" t="s">
-        <v>1066</v>
-      </c>
-      <c r="O20">
-        <v>5566378377</v>
+        <v>1077</v>
+      </c>
+      <c r="O20" t="s">
+        <v>1100</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>1099</v>
+        <v>1120</v>
       </c>
       <c r="Q20" t="s">
-        <v>1114</v>
+        <v>1135</v>
       </c>
       <c r="R20" t="s">
-        <v>1129</v>
+        <v>1149</v>
       </c>
       <c r="S20" t="s">
-        <v>1141</v>
+        <v>1162</v>
       </c>
       <c r="AD20" s="2" t="s">
-        <v>1192</v>
+        <v>1233</v>
       </c>
       <c r="AE20">
         <v>1614859</v>
@@ -12130,29 +12253,29 @@
       <c r="L21" s="2" t="s">
         <v>1030</v>
       </c>
-      <c r="M21">
-        <v>450</v>
+      <c r="M21" t="s">
+        <v>1054</v>
       </c>
       <c r="N21" t="s">
-        <v>1067</v>
-      </c>
-      <c r="O21">
-        <v>575683054</v>
+        <v>1078</v>
+      </c>
+      <c r="O21" t="s">
+        <v>1101</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>1100</v>
+        <v>1121</v>
       </c>
       <c r="Q21" t="s">
-        <v>1115</v>
+        <v>1136</v>
       </c>
       <c r="R21" t="s">
-        <v>1130</v>
+        <v>1150</v>
       </c>
       <c r="S21" t="s">
-        <v>1142</v>
+        <v>1163</v>
       </c>
       <c r="AD21" s="2" t="s">
-        <v>1193</v>
+        <v>1234</v>
       </c>
       <c r="AE21">
         <v>12664</v>
@@ -12180,14 +12303,14 @@
       <c r="L22" s="2" t="s">
         <v>1031</v>
       </c>
-      <c r="M22">
-        <v>20</v>
+      <c r="M22" t="s">
+        <v>1055</v>
       </c>
       <c r="N22" t="s">
-        <v>1068</v>
-      </c>
-      <c r="O22">
-        <v>1733344</v>
+        <v>1079</v>
+      </c>
+      <c r="O22" t="s">
+        <v>1102</v>
       </c>
     </row>
     <row r="23" spans="1:31">
@@ -12215,26 +12338,32 @@
       <c r="L23" s="2" t="s">
         <v>1032</v>
       </c>
-      <c r="M23">
-        <v>160</v>
+      <c r="M23" t="s">
+        <v>1056</v>
       </c>
       <c r="N23" t="s">
-        <v>1069</v>
-      </c>
-      <c r="O23">
-        <v>3976901103</v>
+        <v>1080</v>
+      </c>
+      <c r="O23" t="s">
+        <v>1103</v>
       </c>
       <c r="W23" s="2" t="s">
-        <v>1155</v>
-      </c>
-      <c r="Z23">
-        <v>9835</v>
-      </c>
-      <c r="AA23">
-        <v>4945</v>
+        <v>1176</v>
+      </c>
+      <c r="X23" t="s">
+        <v>1188</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>1200</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>1211</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>1225</v>
       </c>
       <c r="AD23" s="2" t="s">
-        <v>1194</v>
+        <v>1235</v>
       </c>
       <c r="AE23">
         <v>247288</v>
@@ -12265,17 +12394,17 @@
       <c r="L24" s="2" t="s">
         <v>1033</v>
       </c>
-      <c r="M24">
-        <v>503</v>
+      <c r="M24" t="s">
+        <v>1057</v>
       </c>
       <c r="N24" t="s">
-        <v>1070</v>
-      </c>
-      <c r="O24">
-        <v>4291909398</v>
+        <v>1081</v>
+      </c>
+      <c r="O24" t="s">
+        <v>1104</v>
       </c>
       <c r="AD24" s="2" t="s">
-        <v>1195</v>
+        <v>1236</v>
       </c>
       <c r="AE24">
         <v>5733</v>
@@ -12306,26 +12435,32 @@
       <c r="L25" s="2" t="s">
         <v>1034</v>
       </c>
-      <c r="M25">
-        <v>399</v>
+      <c r="M25" t="s">
+        <v>1058</v>
       </c>
       <c r="N25" t="s">
-        <v>1071</v>
-      </c>
-      <c r="O25">
-        <v>2692197</v>
+        <v>1072</v>
+      </c>
+      <c r="O25" t="s">
+        <v>1105</v>
       </c>
       <c r="W25" s="2" t="s">
-        <v>1156</v>
-      </c>
-      <c r="Z25">
-        <v>1021</v>
-      </c>
-      <c r="AA25">
-        <v>3032</v>
+        <v>1177</v>
+      </c>
+      <c r="X25" t="s">
+        <v>1189</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>1201</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>1212</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>1226</v>
       </c>
       <c r="AD25" s="2" t="s">
-        <v>1196</v>
+        <v>1237</v>
       </c>
       <c r="AE25">
         <v>385</v>
@@ -12359,38 +12494,44 @@
       <c r="L26" s="2" t="s">
         <v>1035</v>
       </c>
-      <c r="M26">
-        <v>168</v>
+      <c r="M26" t="s">
+        <v>1059</v>
       </c>
       <c r="N26" t="s">
-        <v>1072</v>
-      </c>
-      <c r="O26">
-        <v>6509411</v>
+        <v>1082</v>
+      </c>
+      <c r="O26" t="s">
+        <v>1106</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>1101</v>
+        <v>1122</v>
       </c>
       <c r="Q26" t="s">
-        <v>1116</v>
+        <v>1137</v>
       </c>
       <c r="R26" t="s">
-        <v>1131</v>
+        <v>1151</v>
       </c>
       <c r="S26" t="s">
-        <v>1143</v>
+        <v>1164</v>
       </c>
       <c r="W26" s="2" t="s">
-        <v>1157</v>
-      </c>
-      <c r="Z26">
-        <v>151</v>
-      </c>
-      <c r="AA26">
-        <v>434</v>
+        <v>1178</v>
+      </c>
+      <c r="X26" t="s">
+        <v>1190</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>1202</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>1213</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>1227</v>
       </c>
       <c r="AD26" s="2" t="s">
-        <v>1197</v>
+        <v>1238</v>
       </c>
       <c r="AE26">
         <v>1538</v>
@@ -12415,17 +12556,17 @@
       <c r="L27" s="2" t="s">
         <v>1036</v>
       </c>
-      <c r="M27">
-        <v>551</v>
+      <c r="M27" t="s">
+        <v>1060</v>
       </c>
       <c r="N27" t="s">
-        <v>1073</v>
-      </c>
-      <c r="O27">
-        <v>37690557</v>
+        <v>1083</v>
+      </c>
+      <c r="O27" t="s">
+        <v>1107</v>
       </c>
       <c r="AD27" s="2" t="s">
-        <v>1198</v>
+        <v>1239</v>
       </c>
       <c r="AE27">
         <v>362</v>
@@ -12459,14 +12600,14 @@
       <c r="L28" s="2" t="s">
         <v>1037</v>
       </c>
-      <c r="M28">
-        <v>485</v>
+      <c r="M28" t="s">
+        <v>1061</v>
       </c>
       <c r="N28" t="s">
-        <v>1074</v>
-      </c>
-      <c r="O28">
-        <v>5220533590</v>
+        <v>1084</v>
+      </c>
+      <c r="O28" t="s">
+        <v>1108</v>
       </c>
     </row>
     <row r="29" spans="1:31">

</xml_diff>